<commit_message>
calculate invoices right, add card_number as unique for each invoice
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -635,13 +635,13 @@
   </sheetPr>
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C28" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N28" activeCellId="0" sqref="N28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B11" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="26.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="19.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.66"/>

</xml_diff>